<commit_message>
Fix: Bug na linha 34
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Plan1"/>
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
-  <si>
-    <t/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Nome Fantasia</t>
   </si>
@@ -69,12 +66,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -384,36 +378,34 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="33.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="28.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="29.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="33.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="28.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="29.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -427,13 +419,13 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -444,9 +436,7 @@
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>